<commit_message>
correct some dependencies, code cleanup
</commit_message>
<xml_diff>
--- a/Databank.xlsx
+++ b/Databank.xlsx
@@ -4478,110 +4478,152 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>De Havilland</t>
+          <t>Embraer</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Comet 1</t>
+          <t>Embraer 190</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1952</v>
-      </c>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
+        <v>2004</v>
+      </c>
+      <c r="E52" t="n">
+        <v>51843.125</v>
+      </c>
+      <c r="F52" t="n">
+        <v>44140.625</v>
+      </c>
       <c r="G52" t="n">
-        <v>44</v>
-      </c>
-      <c r="H52" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="H52" t="n">
+        <v>16347.75</v>
+      </c>
       <c r="I52" t="n">
-        <v>28.9</v>
+        <v>16.77016917536357</v>
       </c>
       <c r="J52" t="n">
-        <v>0.1956844519784796</v>
+        <v>0.3392881252903102</v>
       </c>
       <c r="K52" t="n">
-        <v>8.624957727272728</v>
+        <v>1.712372106412916</v>
       </c>
       <c r="L52" t="n">
-        <v>721.5909090909091</v>
-      </c>
-      <c r="M52" t="n">
-        <v>13.03220058392828</v>
-      </c>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+        <v>226.7204301075269</v>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>9.754665681149657</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.04141733060561711</v>
+      </c>
+      <c r="P52" t="n">
+        <v>30.545</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.7117598908588553</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0.4763098239510975</v>
+      </c>
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr"/>
-      <c r="X52" t="inlineStr"/>
-      <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>99</v>
+      </c>
+      <c r="X52" t="n">
+        <v>10.605</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>7.026875</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>61088.37579710694</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>De Havilland</t>
+          <t>Embraer</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Comet 4</t>
+          <t>Embraer-135</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>1958</v>
-      </c>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
+        <v>1999</v>
+      </c>
+      <c r="E53" t="n">
+        <v>21096</v>
+      </c>
+      <c r="F53" t="n">
+        <v>15840</v>
+      </c>
       <c r="G53" t="n">
-        <v>109</v>
-      </c>
-      <c r="H53" t="inlineStr"/>
+        <v>37</v>
+      </c>
+      <c r="H53" t="n">
+        <v>8216.799999999999</v>
+      </c>
       <c r="I53" t="n">
-        <v>26.4</v>
+        <v>18.16621531661354</v>
       </c>
       <c r="J53" t="n">
-        <v>0.2142151765976538</v>
-      </c>
-      <c r="K53" t="n">
-        <v>3.451363636363636</v>
-      </c>
+        <v>0.3113135990720869</v>
+      </c>
+      <c r="K53" t="inlineStr"/>
       <c r="L53" t="n">
-        <v>313.8715596330275</v>
-      </c>
-      <c r="M53" t="n">
-        <v>12.94289328120862</v>
-      </c>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
+        <v>339.1891891891892</v>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="n">
+        <v>7.846846424384525</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.05070665796303604</v>
+      </c>
+      <c r="P53" t="n">
+        <v>20.04</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0.5827229105762763</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0.5342456021720363</v>
+      </c>
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
-      <c r="Y53" t="inlineStr"/>
-      <c r="Z53" t="inlineStr"/>
+      <c r="W53" t="n">
+        <v>37</v>
+      </c>
+      <c r="X53" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>4.762</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>49755.49877845949</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4591,7 +4633,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Embraer 190</t>
+          <t>Embraer-140</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -4600,74 +4642,44 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2004</v>
-      </c>
-      <c r="E54" t="n">
-        <v>51843.125</v>
-      </c>
-      <c r="F54" t="n">
-        <v>44140.625</v>
-      </c>
+        <v>2001</v>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>124</v>
-      </c>
-      <c r="H54" t="n">
-        <v>16347.75</v>
-      </c>
-      <c r="I54" t="n">
-        <v>16.77016917536357</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0.3392881252903102</v>
-      </c>
-      <c r="K54" t="n">
-        <v>1.712372106412916</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
       <c r="L54" t="n">
-        <v>226.7204301075269</v>
+        <v>268.1818181818182</v>
       </c>
       <c r="M54" t="inlineStr"/>
-      <c r="N54" t="n">
-        <v>9.754665681149657</v>
-      </c>
-      <c r="O54" t="n">
-        <v>0.04141733060561711</v>
-      </c>
-      <c r="P54" t="n">
-        <v>30.545</v>
-      </c>
-      <c r="Q54" t="n">
-        <v>0.7117598908588553</v>
-      </c>
-      <c r="R54" t="n">
-        <v>0.4763098239510975</v>
-      </c>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr"/>
-      <c r="W54" t="n">
-        <v>99</v>
-      </c>
-      <c r="X54" t="n">
-        <v>10.605</v>
-      </c>
-      <c r="Y54" t="n">
-        <v>7.026875</v>
-      </c>
-      <c r="Z54" t="n">
-        <v>61088.37579710694</v>
-      </c>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Embraer</t>
+          <t xml:space="preserve">Embraer </t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Embraer-135</t>
+          <t>EMB-120 Brasilia</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -4676,72 +4688,44 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1999</v>
-      </c>
-      <c r="E55" t="n">
-        <v>21096</v>
-      </c>
-      <c r="F55" t="n">
-        <v>15840</v>
-      </c>
+        <v>1985</v>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
-        <v>37</v>
-      </c>
-      <c r="H55" t="n">
-        <v>8216.799999999999</v>
-      </c>
-      <c r="I55" t="n">
-        <v>18.16621531661354</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0.3113135990720869</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="n">
-        <v>339.1891891891892</v>
+        <v>252</v>
       </c>
       <c r="M55" t="inlineStr"/>
-      <c r="N55" t="n">
-        <v>7.846846424384525</v>
-      </c>
-      <c r="O55" t="n">
-        <v>0.05070665796303604</v>
-      </c>
-      <c r="P55" t="n">
-        <v>20.04</v>
-      </c>
-      <c r="Q55" t="n">
-        <v>0.5827229105762763</v>
-      </c>
-      <c r="R55" t="n">
-        <v>0.5342456021720363</v>
-      </c>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr"/>
-      <c r="W55" t="n">
-        <v>37</v>
-      </c>
-      <c r="X55" t="n">
-        <v>6.76</v>
-      </c>
-      <c r="Y55" t="n">
-        <v>4.762</v>
-      </c>
-      <c r="Z55" t="n">
-        <v>49755.49877845949</v>
-      </c>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Embraer</t>
+          <t xml:space="preserve">Embraer </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Embraer-140</t>
+          <t>Embraer ERJ-175</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -4750,34 +4734,64 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2001</v>
-      </c>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
+        <v>2005</v>
+      </c>
+      <c r="E56" t="n">
+        <v>37500</v>
+      </c>
+      <c r="F56" t="n">
+        <v>31700</v>
+      </c>
       <c r="G56" t="n">
-        <v>44</v>
-      </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
+        <v>88</v>
+      </c>
+      <c r="H56" t="n">
+        <v>11625</v>
+      </c>
+      <c r="I56" t="n">
+        <v>18.19340342917936</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.3108455349745253</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1.528589461364119</v>
+      </c>
       <c r="L56" t="n">
-        <v>268.1818181818182</v>
+        <v>247.8409090909091</v>
       </c>
       <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
+      <c r="N56" t="n">
+        <v>11.28743811881188</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.03525045750342684</v>
+      </c>
+      <c r="P56" t="n">
+        <v>28.65</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.7270491548603031</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0.4275455547427663</v>
+      </c>
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
+      <c r="W56" t="n">
+        <v>75</v>
+      </c>
+      <c r="X56" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>37180.61653102213</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4787,7 +4801,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>EMB-120 Brasilia</t>
+          <t>Embraer-145</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -4796,44 +4810,74 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1985</v>
-      </c>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
+        <v>1996</v>
+      </c>
+      <c r="E57" t="n">
+        <v>20016.66666666667</v>
+      </c>
+      <c r="F57" t="n">
+        <v>17333.33333333333</v>
+      </c>
       <c r="G57" t="n">
-        <v>30</v>
-      </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="H57" t="n">
+        <v>5528</v>
+      </c>
+      <c r="I57" t="n">
+        <v>18.22195069609804</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.3103601476304506</v>
+      </c>
+      <c r="K57" t="n">
+        <v>2.103581856805667</v>
+      </c>
       <c r="L57" t="n">
-        <v>252</v>
+        <v>244.1333333333333</v>
       </c>
       <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="N57" t="n">
+        <v>7.975146541617818</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.04995164617426398</v>
+      </c>
+      <c r="P57" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.6081109382651159</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0.5103718988149327</v>
+      </c>
       <c r="S57" t="inlineStr"/>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr"/>
-      <c r="Z57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>50</v>
+      </c>
+      <c r="X57" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>4.837777777777777</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>44777.31705387121</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Embraer </t>
+          <t xml:space="preserve">Fokker </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Embraer ERJ-175</t>
+          <t>Fokker 100</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -4842,74 +4886,44 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2005</v>
-      </c>
-      <c r="E58" t="n">
-        <v>37500</v>
-      </c>
-      <c r="F58" t="n">
-        <v>31700</v>
-      </c>
+        <v>1988</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
-        <v>88</v>
-      </c>
-      <c r="H58" t="n">
-        <v>11625</v>
-      </c>
-      <c r="I58" t="n">
-        <v>18.19340342917936</v>
-      </c>
-      <c r="J58" t="n">
-        <v>0.3108455349745253</v>
-      </c>
-      <c r="K58" t="n">
-        <v>1.528589461364119</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
       <c r="L58" t="n">
-        <v>247.8409090909091</v>
+        <v>202.3142076502733</v>
       </c>
       <c r="M58" t="inlineStr"/>
-      <c r="N58" t="n">
-        <v>11.28743811881188</v>
-      </c>
-      <c r="O58" t="n">
-        <v>0.03525045750342684</v>
-      </c>
-      <c r="P58" t="n">
-        <v>28.65</v>
-      </c>
-      <c r="Q58" t="n">
-        <v>0.7270491548603031</v>
-      </c>
-      <c r="R58" t="n">
-        <v>0.4275455547427663</v>
-      </c>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr"/>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr"/>
-      <c r="W58" t="n">
-        <v>75</v>
-      </c>
-      <c r="X58" t="n">
-        <v>9.82</v>
-      </c>
-      <c r="Y58" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="Z58" t="n">
-        <v>37180.61653102213</v>
-      </c>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
+      <c r="Z58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Embraer </t>
+          <t xml:space="preserve">Gates Learjet </t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Embraer-145</t>
+          <t>Lear-31/35/36</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -4918,138 +4932,134 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E59" t="n">
-        <v>20016.66666666667</v>
-      </c>
-      <c r="F59" t="n">
-        <v>17333.33333333333</v>
-      </c>
-      <c r="G59" t="n">
-        <v>50</v>
-      </c>
-      <c r="H59" t="n">
-        <v>5528</v>
-      </c>
-      <c r="I59" t="n">
-        <v>18.22195069609804</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0.3103601476304506</v>
-      </c>
-      <c r="K59" t="n">
-        <v>2.103581856805667</v>
-      </c>
-      <c r="L59" t="n">
-        <v>244.1333333333333</v>
-      </c>
+        <v>1974</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
-      <c r="N59" t="n">
-        <v>7.975146541617818</v>
-      </c>
-      <c r="O59" t="n">
-        <v>0.04995164617426398</v>
-      </c>
-      <c r="P59" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="Q59" t="n">
-        <v>0.6081109382651159</v>
-      </c>
-      <c r="R59" t="n">
-        <v>0.5103718988149327</v>
-      </c>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr"/>
-      <c r="W59" t="n">
-        <v>50</v>
-      </c>
-      <c r="X59" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="Y59" t="n">
-        <v>4.837777777777777</v>
-      </c>
-      <c r="Z59" t="n">
-        <v>44777.31705387121</v>
-      </c>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
+      <c r="Z59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fokker </t>
+          <t>Lockheed</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Fokker 100</t>
+          <t>L1011-1/100/200</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1988</v>
-      </c>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
+        <v>1973</v>
+      </c>
+      <c r="E60" t="n">
+        <v>224982</v>
+      </c>
+      <c r="F60" t="n">
+        <v>153314</v>
+      </c>
       <c r="G60" t="n">
-        <v>122</v>
-      </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr"/>
+        <v>400</v>
+      </c>
+      <c r="H60" t="n">
+        <v>120705</v>
+      </c>
+      <c r="I60" t="n">
+        <v>17.5682</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.3219043875967976</v>
+      </c>
+      <c r="K60" t="n">
+        <v>1.69015679246197</v>
+      </c>
       <c r="L60" t="n">
-        <v>202.3142076502733</v>
-      </c>
-      <c r="M60" t="inlineStr"/>
+        <v>277.7625</v>
+      </c>
+      <c r="M60" t="n">
+        <v>14.3153</v>
+      </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr"/>
-      <c r="R60" t="inlineStr"/>
+      <c r="Q60" t="n">
+        <v>0.7611246338515383</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.4229325570082481</v>
+      </c>
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr"/>
-      <c r="W60" t="inlineStr"/>
+      <c r="W60" t="n">
+        <v>314</v>
+      </c>
       <c r="X60" t="inlineStr"/>
-      <c r="Y60" t="inlineStr"/>
-      <c r="Z60" t="inlineStr"/>
+      <c r="Y60" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>163349.5957069433</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gates Learjet </t>
+          <t xml:space="preserve">Lockheed </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lear-31/35/36</t>
+          <t>L1011-500</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1974</v>
+        <v>1979</v>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>330</v>
+      </c>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr"/>
+      <c r="K61" t="n">
+        <v>1.8209</v>
+      </c>
+      <c r="L61" t="n">
+        <v>330.0757575757576</v>
+      </c>
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
@@ -5068,12 +5078,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Lockheed</t>
+          <t>McDonnell Douglas</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>L1011-1/100/200</t>
+          <t>DC10-30</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -5082,68 +5092,56 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>1973</v>
-      </c>
-      <c r="E62" t="n">
-        <v>224982</v>
-      </c>
-      <c r="F62" t="n">
-        <v>153314</v>
-      </c>
+        <v>1972</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
-        <v>400</v>
-      </c>
-      <c r="H62" t="n">
-        <v>120705</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="H62" t="inlineStr"/>
       <c r="I62" t="n">
-        <v>17.5682</v>
+        <v>17.7708</v>
       </c>
       <c r="J62" t="n">
-        <v>0.3219043875967976</v>
+        <v>0.3182344442668905</v>
       </c>
       <c r="K62" t="n">
-        <v>1.69015679246197</v>
+        <v>1.803152741832779</v>
       </c>
       <c r="L62" t="n">
-        <v>277.7625</v>
+        <v>318.9342105263158</v>
       </c>
       <c r="M62" t="n">
-        <v>14.3153</v>
+        <v>15.2348</v>
       </c>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="n">
-        <v>0.7611246338515383</v>
-      </c>
-      <c r="R62" t="n">
-        <v>0.4229325570082481</v>
-      </c>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
       <c r="S62" t="inlineStr"/>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr"/>
       <c r="W62" t="n">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="X62" t="inlineStr"/>
-      <c r="Y62" t="n">
-        <v>4.54</v>
-      </c>
+      <c r="Y62" t="inlineStr"/>
       <c r="Z62" t="n">
-        <v>163349.5957069433</v>
+        <v>176259.1642868837</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lockheed </t>
+          <t>McDonnell Douglas</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>L1011-500</t>
+          <t>DC10-40</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -5152,36 +5150,58 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>1979</v>
-      </c>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+        <v>1972</v>
+      </c>
+      <c r="E63" t="n">
+        <v>256280</v>
+      </c>
+      <c r="F63" t="n">
+        <v>177355</v>
+      </c>
       <c r="G63" t="n">
-        <v>330</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
+        <v>380</v>
+      </c>
+      <c r="H63" t="n">
+        <v>137520</v>
+      </c>
+      <c r="I63" t="n">
+        <v>17.4331</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.3243990261157257</v>
+      </c>
       <c r="K63" t="n">
-        <v>1.8209</v>
+        <v>1.815799269772046</v>
       </c>
       <c r="L63" t="n">
-        <v>330.0757575757576</v>
-      </c>
-      <c r="M63" t="inlineStr"/>
+        <v>323.5526315789473</v>
+      </c>
+      <c r="M63" t="n">
+        <v>13.9129</v>
+      </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
-      <c r="Q63" t="inlineStr"/>
-      <c r="R63" t="inlineStr"/>
+      <c r="Q63" t="n">
+        <v>0.7498489997700178</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.4326919339257812</v>
+      </c>
       <c r="S63" t="inlineStr"/>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr"/>
+      <c r="W63" t="n">
+        <v>292</v>
+      </c>
       <c r="X63" t="inlineStr"/>
-      <c r="Y63" t="inlineStr"/>
-      <c r="Z63" t="inlineStr"/>
+      <c r="Y63" t="n">
+        <v>4.961538461538462</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>176295.7276686124</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5191,41 +5211,49 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DC10-30</t>
+          <t>DC9-30</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>1972</v>
-      </c>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
+        <v>1966</v>
+      </c>
+      <c r="E64" t="n">
+        <v>47627</v>
+      </c>
+      <c r="F64" t="n">
+        <v>39463</v>
+      </c>
       <c r="G64" t="n">
-        <v>380</v>
-      </c>
-      <c r="H64" t="inlineStr"/>
+        <v>127</v>
+      </c>
+      <c r="H64" t="n">
+        <v>13926</v>
+      </c>
       <c r="I64" t="n">
-        <v>17.7708</v>
+        <v>22.4331</v>
       </c>
       <c r="J64" t="n">
-        <v>0.3182344442668905</v>
+        <v>0.2520953707770241</v>
       </c>
       <c r="K64" t="n">
-        <v>1.803152741832779</v>
+        <v>2.396593879999583</v>
       </c>
       <c r="L64" t="n">
-        <v>318.9342105263158</v>
+        <v>203.0629921259843</v>
       </c>
       <c r="M64" t="n">
-        <v>15.2348</v>
+        <v>13.798</v>
       </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
-      <c r="P64" t="inlineStr"/>
+      <c r="P64" t="n">
+        <v>28.44</v>
+      </c>
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr"/>
@@ -5233,12 +5261,16 @@
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
       <c r="W64" t="n">
-        <v>266</v>
-      </c>
-      <c r="X64" t="inlineStr"/>
-      <c r="Y64" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="X64" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>1.038181818181818</v>
+      </c>
       <c r="Z64" t="n">
-        <v>176259.1642868837</v>
+        <v>50239.33056833609</v>
       </c>
     </row>
     <row r="65">
@@ -5249,67 +5281,61 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DC10-40</t>
+          <t>DC9-40</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1972</v>
+        <v>1968</v>
       </c>
       <c r="E65" t="n">
-        <v>256280</v>
+        <v>51710</v>
       </c>
       <c r="F65" t="n">
-        <v>177355</v>
+        <v>42184</v>
       </c>
       <c r="G65" t="n">
-        <v>380</v>
+        <v>128</v>
       </c>
       <c r="H65" t="n">
-        <v>137520</v>
+        <v>13926</v>
       </c>
       <c r="I65" t="n">
-        <v>17.4331</v>
+        <v>22.98764963035378</v>
       </c>
       <c r="J65" t="n">
-        <v>0.3243990261157257</v>
+        <v>0.2460964991804533</v>
       </c>
       <c r="K65" t="n">
-        <v>1.815799269772046</v>
+        <v>2.0777</v>
       </c>
       <c r="L65" t="n">
-        <v>323.5526315789473</v>
-      </c>
-      <c r="M65" t="n">
-        <v>13.9129</v>
-      </c>
+        <v>217.3515625</v>
+      </c>
+      <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
-      <c r="P65" t="inlineStr"/>
-      <c r="Q65" t="n">
-        <v>0.7498489997700178</v>
-      </c>
-      <c r="R65" t="n">
-        <v>0.4326919339257812</v>
-      </c>
+      <c r="P65" t="n">
+        <v>28.44</v>
+      </c>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
       <c r="S65" t="inlineStr"/>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
-      <c r="W65" t="n">
-        <v>292</v>
-      </c>
-      <c r="X65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="n">
+        <v>8.5</v>
+      </c>
       <c r="Y65" t="n">
-        <v>4.961538461538462</v>
-      </c>
-      <c r="Z65" t="n">
-        <v>176295.7276686124</v>
-      </c>
+        <v>1.036428571428571</v>
+      </c>
+      <c r="Z65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5319,7 +5345,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>DC9-30</t>
+          <t>DC9-50</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -5328,39 +5354,37 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1966</v>
+        <v>1976</v>
       </c>
       <c r="E66" t="n">
-        <v>47627</v>
+        <v>54885</v>
       </c>
       <c r="F66" t="n">
-        <v>39463</v>
+        <v>44679</v>
       </c>
       <c r="G66" t="n">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="H66" t="n">
         <v>13926</v>
       </c>
       <c r="I66" t="n">
-        <v>22.4331</v>
+        <v>23.15547775838727</v>
       </c>
       <c r="J66" t="n">
-        <v>0.2520953707770241</v>
+        <v>0.2443182490108967</v>
       </c>
       <c r="K66" t="n">
-        <v>2.396593879999583</v>
+        <v>2.1014</v>
       </c>
       <c r="L66" t="n">
-        <v>203.0629921259843</v>
-      </c>
-      <c r="M66" t="n">
-        <v>13.798</v>
-      </c>
+        <v>211.0503597122302</v>
+      </c>
+      <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="n">
-        <v>28.44</v>
+        <v>28.45</v>
       </c>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
@@ -5368,18 +5392,14 @@
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
-      <c r="W66" t="n">
-        <v>100</v>
-      </c>
+      <c r="W66" t="inlineStr"/>
       <c r="X66" t="n">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="Y66" t="n">
-        <v>1.038181818181818</v>
-      </c>
-      <c r="Z66" t="n">
-        <v>50239.33056833609</v>
-      </c>
+        <v>1.04375</v>
+      </c>
+      <c r="Z66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5389,7 +5409,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DC9-40</t>
+          <t>MD-90</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -5398,52 +5418,62 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>1968</v>
+        <v>1995</v>
       </c>
       <c r="E67" t="n">
-        <v>51710</v>
+        <v>70760</v>
       </c>
       <c r="F67" t="n">
-        <v>42184</v>
+        <v>58967</v>
       </c>
       <c r="G67" t="n">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="H67" t="n">
-        <v>13926</v>
+        <v>22104</v>
       </c>
       <c r="I67" t="n">
-        <v>22.98764963035378</v>
+        <v>16.99770822716683</v>
       </c>
       <c r="J67" t="n">
-        <v>0.2460964991804533</v>
+        <v>0.3327206303053079</v>
       </c>
       <c r="K67" t="n">
-        <v>2.0777</v>
+        <v>1.340189934684793</v>
       </c>
       <c r="L67" t="n">
-        <v>217.3515625</v>
-      </c>
-      <c r="M67" t="inlineStr"/>
+        <v>242.5489021956088</v>
+      </c>
+      <c r="M67" t="n">
+        <v>12.54450404243209</v>
+      </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="n">
-        <v>28.44</v>
-      </c>
-      <c r="Q67" t="inlineStr"/>
-      <c r="R67" t="inlineStr"/>
+        <v>32.87</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0.7458748318947507</v>
+      </c>
+      <c r="R67" t="n">
+        <v>0.4460862698857084</v>
+      </c>
       <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
-      <c r="W67" t="inlineStr"/>
+      <c r="W67" t="n">
+        <v>148</v>
+      </c>
       <c r="X67" t="n">
-        <v>8.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="Y67" t="n">
-        <v>1.036428571428571</v>
-      </c>
-      <c r="Z67" t="inlineStr"/>
+        <v>4.74</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>63894.06446530207</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5453,7 +5483,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DC9-50</t>
+          <t>MD80/DC9-80</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -5462,136 +5492,138 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1976</v>
+        <v>1980</v>
       </c>
       <c r="E68" t="n">
-        <v>54885</v>
+        <v>66170.71428571429</v>
       </c>
       <c r="F68" t="n">
-        <v>44679</v>
+        <v>54258.33333333334</v>
       </c>
       <c r="G68" t="n">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="H68" t="n">
-        <v>13926</v>
+        <v>22128.57142857143</v>
       </c>
       <c r="I68" t="n">
-        <v>23.15547775838727</v>
+        <v>20.744</v>
       </c>
       <c r="J68" t="n">
-        <v>0.2443182490108967</v>
+        <v>0.2726224769657761</v>
       </c>
       <c r="K68" t="n">
-        <v>2.1014</v>
+        <v>1.654110373626076</v>
       </c>
       <c r="L68" t="n">
-        <v>211.0503597122302</v>
-      </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr"/>
+        <v>201.4290697674419</v>
+      </c>
+      <c r="M68" t="n">
+        <v>13.9129</v>
+      </c>
+      <c r="N68" t="n">
+        <v>9.609283170080145</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0.04140655974928667</v>
+      </c>
       <c r="P68" t="n">
-        <v>28.45</v>
+        <v>32.85</v>
       </c>
       <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr"/>
-      <c r="S68" t="inlineStr"/>
-      <c r="T68" t="inlineStr"/>
-      <c r="U68" t="inlineStr"/>
-      <c r="V68" t="inlineStr"/>
-      <c r="W68" t="inlineStr"/>
+      <c r="S68" t="n">
+        <v>0.4818759914491247</v>
+      </c>
+      <c r="T68" t="n">
+        <v>0.04330909613574976</v>
+      </c>
+      <c r="U68" t="n">
+        <v>0.009614788308106073</v>
+      </c>
+      <c r="V68" t="n">
+        <v>0.03369430782764369</v>
+      </c>
+      <c r="W68" t="n">
+        <v>144</v>
+      </c>
       <c r="X68" t="n">
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="Y68" t="n">
-        <v>1.04375</v>
-      </c>
-      <c r="Z68" t="inlineStr"/>
+        <v>1.725714285714286</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>58284.64332602391</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>McDonnell Douglas</t>
+          <t xml:space="preserve">McDonnell Douglas </t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MD-90</t>
+          <t>DC10-10</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1995</v>
-      </c>
-      <c r="E69" t="n">
-        <v>70760</v>
-      </c>
-      <c r="F69" t="n">
-        <v>58967</v>
-      </c>
+        <v>1970</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
       <c r="G69" t="n">
-        <v>167</v>
-      </c>
-      <c r="H69" t="n">
-        <v>22104</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="H69" t="inlineStr"/>
       <c r="I69" t="n">
-        <v>16.99770822716683</v>
+        <v>17.0953</v>
       </c>
       <c r="J69" t="n">
-        <v>0.3327206303053079</v>
+        <v>0.3308090915150982</v>
       </c>
       <c r="K69" t="n">
-        <v>1.340189934684793</v>
+        <v>1.665838405572881</v>
       </c>
       <c r="L69" t="n">
-        <v>242.5489021956088</v>
+        <v>286.6842105263158</v>
       </c>
       <c r="M69" t="n">
-        <v>12.54450404243209</v>
+        <v>14.2003</v>
       </c>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
-      <c r="P69" t="n">
-        <v>32.87</v>
-      </c>
-      <c r="Q69" t="n">
-        <v>0.7458748318947507</v>
-      </c>
-      <c r="R69" t="n">
-        <v>0.4460862698857084</v>
-      </c>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="inlineStr"/>
       <c r="S69" t="inlineStr"/>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
       <c r="W69" t="n">
-        <v>148</v>
-      </c>
-      <c r="X69" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="Y69" t="n">
-        <v>4.74</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
       <c r="Z69" t="n">
-        <v>63894.06446530207</v>
+        <v>169567.8746222493</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>McDonnell Douglas</t>
+          <t xml:space="preserve">McDonnell Douglas </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>MD80/DC9-80</t>
+          <t>DC9-10</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -5600,70 +5632,52 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>1980</v>
+        <v>1965</v>
       </c>
       <c r="E70" t="n">
-        <v>66170.71428571429</v>
+        <v>41141</v>
       </c>
       <c r="F70" t="n">
-        <v>54258.33333333334</v>
+        <v>33566</v>
       </c>
       <c r="G70" t="n">
-        <v>172</v>
+        <v>109</v>
       </c>
       <c r="H70" t="n">
-        <v>22128.57142857143</v>
+        <v>13979</v>
       </c>
       <c r="I70" t="n">
-        <v>20.744</v>
+        <v>22.88492472710245</v>
       </c>
       <c r="J70" t="n">
-        <v>0.2726224769657761</v>
+        <v>0.2472409829726473</v>
       </c>
       <c r="K70" t="n">
-        <v>1.654110373626076</v>
+        <v>2.9899</v>
       </c>
       <c r="L70" t="n">
-        <v>201.4290697674419</v>
-      </c>
-      <c r="M70" t="n">
-        <v>13.9129</v>
-      </c>
-      <c r="N70" t="n">
-        <v>9.609283170080145</v>
-      </c>
-      <c r="O70" t="n">
-        <v>0.04140655974928667</v>
-      </c>
+        <v>204.5871559633028</v>
+      </c>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
       <c r="P70" t="n">
-        <v>32.85</v>
+        <v>27.25</v>
       </c>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
-      <c r="S70" t="n">
-        <v>0.4818759914491247</v>
-      </c>
-      <c r="T70" t="n">
-        <v>0.04330909613574976</v>
-      </c>
-      <c r="U70" t="n">
-        <v>0.009614788308106073</v>
-      </c>
-      <c r="V70" t="n">
-        <v>0.03369430782764369</v>
-      </c>
-      <c r="W70" t="n">
-        <v>144</v>
-      </c>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
       <c r="X70" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="Y70" t="n">
-        <v>1.725714285714286</v>
-      </c>
-      <c r="Z70" t="n">
-        <v>58284.64332602391</v>
-      </c>
+        <v>1.032222222222222</v>
+      </c>
+      <c r="Z70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5673,7 +5687,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DC10-10</t>
+          <t>MD-11</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -5682,96 +5696,94 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
+        <v>1990</v>
+      </c>
+      <c r="E71" t="n">
+        <v>276691</v>
+      </c>
+      <c r="F71" t="n">
+        <v>195045</v>
+      </c>
       <c r="G71" t="n">
-        <v>380</v>
-      </c>
-      <c r="H71" t="inlineStr"/>
+        <v>410</v>
+      </c>
+      <c r="H71" t="n">
+        <v>144782</v>
+      </c>
       <c r="I71" t="n">
-        <v>17.0953</v>
+        <v>17.17456583460847</v>
       </c>
       <c r="J71" t="n">
-        <v>0.3308090915150982</v>
+        <v>0.329294025279972</v>
       </c>
       <c r="K71" t="n">
-        <v>1.665838405572881</v>
+        <v>1.744608638314735</v>
       </c>
       <c r="L71" t="n">
-        <v>286.6842105263158</v>
+        <v>317.4756097560976</v>
       </c>
       <c r="M71" t="n">
-        <v>14.2003</v>
+        <v>17.18295849059495</v>
       </c>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr"/>
-      <c r="R71" t="inlineStr"/>
+      <c r="Q71" t="n">
+        <v>0.7918255422774546</v>
+      </c>
+      <c r="R71" t="n">
+        <v>0.4158827258454688</v>
+      </c>
       <c r="S71" t="inlineStr"/>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr"/>
       <c r="W71" t="n">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="X71" t="inlineStr"/>
-      <c r="Y71" t="inlineStr"/>
+      <c r="Y71" t="n">
+        <v>4.8</v>
+      </c>
       <c r="Z71" t="n">
-        <v>169567.8746222493</v>
+        <v>160911.0912490309</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t xml:space="preserve">McDonnell Douglas </t>
+          <t xml:space="preserve">Saab-Fairchild </t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DC9-10</t>
+          <t>340/B</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>1965</v>
-      </c>
-      <c r="E72" t="n">
-        <v>41141</v>
-      </c>
-      <c r="F72" t="n">
-        <v>33566</v>
-      </c>
+        <v>1984</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
       <c r="G72" t="n">
-        <v>109</v>
-      </c>
-      <c r="H72" t="n">
-        <v>13979</v>
-      </c>
-      <c r="I72" t="n">
-        <v>22.88492472710245</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0.2472409829726473</v>
-      </c>
-      <c r="K72" t="n">
-        <v>2.9899</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
       <c r="L72" t="n">
-        <v>204.5871559633028</v>
+        <v>241.9117647058823</v>
       </c>
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
-      <c r="P72" t="n">
-        <v>27.25</v>
-      </c>
+      <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
       <c r="S72" t="inlineStr"/>
@@ -5779,116 +5791,104 @@
       <c r="U72" t="inlineStr"/>
       <c r="V72" t="inlineStr"/>
       <c r="W72" t="inlineStr"/>
-      <c r="X72" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="Y72" t="n">
-        <v>1.032222222222222</v>
-      </c>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
       <c r="Z72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t xml:space="preserve">McDonnell Douglas </t>
+          <t>de Havilland</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>MD-11</t>
+          <t>Comet 1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1990</v>
-      </c>
-      <c r="E73" t="n">
-        <v>276691</v>
-      </c>
-      <c r="F73" t="n">
-        <v>195045</v>
-      </c>
+        <v>1952</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
       <c r="G73" t="n">
-        <v>410</v>
-      </c>
-      <c r="H73" t="n">
-        <v>144782</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
-        <v>17.17456583460847</v>
+        <v>28.9</v>
       </c>
       <c r="J73" t="n">
-        <v>0.329294025279972</v>
+        <v>0.1956844519784796</v>
       </c>
       <c r="K73" t="n">
-        <v>1.744608638314735</v>
+        <v>8.624957727272728</v>
       </c>
       <c r="L73" t="n">
-        <v>317.4756097560976</v>
+        <v>721.5909090909091</v>
       </c>
       <c r="M73" t="n">
-        <v>17.18295849059495</v>
+        <v>13.03220058392828</v>
       </c>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
-      <c r="Q73" t="n">
-        <v>0.7918255422774546</v>
-      </c>
-      <c r="R73" t="n">
-        <v>0.4158827258454688</v>
-      </c>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
       <c r="S73" t="inlineStr"/>
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
       <c r="V73" t="inlineStr"/>
-      <c r="W73" t="n">
-        <v>254</v>
-      </c>
+      <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr"/>
-      <c r="Y73" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="Z73" t="n">
-        <v>160911.0912490309</v>
-      </c>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Saab-Fairchild </t>
+          <t>de Havilland</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>340/B</t>
+          <t>Comet 4</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>1984</v>
+        <v>1958</v>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="n">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr"/>
+      <c r="I74" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.2142151765976538</v>
+      </c>
+      <c r="K74" t="n">
+        <v>3.451363636363636</v>
+      </c>
       <c r="L74" t="n">
-        <v>241.9117647058823</v>
-      </c>
-      <c r="M74" t="inlineStr"/>
+        <v>313.8715596330275</v>
+      </c>
+      <c r="M74" t="n">
+        <v>12.94289328120862</v>
+      </c>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>

</xml_diff>